<commit_message>
Ejecución de PF Alta Coche. Corrijo patrón expresión regular de validación de la matricula.
</commit_message>
<xml_diff>
--- a/doc/Pruebas Funcionales/Documento PF.xlsx
+++ b/doc/Pruebas Funcionales/Documento PF.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4420"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Casos" sheetId="1" r:id="rId1"/>
+    <sheet name="1.1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>#prueba</t>
   </si>
@@ -38,9 +39,6 @@
     <t>Alta coche</t>
   </si>
   <si>
-    <t>Datos no cumplen validaciones</t>
-  </si>
-  <si>
     <t>Coche ya existe</t>
   </si>
   <si>
@@ -48,6 +46,24 @@
   </si>
   <si>
     <t>Resultado</t>
+  </si>
+  <si>
+    <t>Evidencias</t>
+  </si>
+  <si>
+    <t>Datos no cumplen validaciones: Matricula</t>
+  </si>
+  <si>
+    <t>Patron ^\d{4}[a-bA-B]{3}$</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>Datos no cumplen validaciones: Kilometraje</t>
   </si>
 </sst>
 </file>
@@ -71,7 +87,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -94,13 +110,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -116,6 +184,163 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>156741</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1530350" y="482600"/>
+          <a:ext cx="1439441" cy="768350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>355601</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>25401</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>82219</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3168651" y="520700"/>
+          <a:ext cx="1193800" cy="666419"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>13179</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="69850" y="520700"/>
+          <a:ext cx="1232379" cy="704850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>155697</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagen 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4521200" y="584200"/>
+          <a:ext cx="1212850" cy="676397"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -381,22 +606,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D17"/>
+  <dimension ref="A2:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="27.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.90625" style="6"/>
+    <col min="3" max="3" width="38.26953125" customWidth="1"/>
+    <col min="4" max="4" width="27.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -405,116 +632,210 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
-        <v>1</v>
+      <c r="B3" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2</v>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="5"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="3"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="3"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="5"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="3"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="3"/>
+      <c r="B11" s="5">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="B13" s="5"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="B14" s="5"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+      <c r="B15" s="5"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="B16" s="5"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="B17" s="5"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="1"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="1"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="1"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="1"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="1"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="1"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:A12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pasadas las PF de Alta Coche.
</commit_message>
<xml_diff>
--- a/doc/Pruebas Funcionales/Documento PF.xlsx
+++ b/doc/Pruebas Funcionales/Documento PF.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4420" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4420" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Casos" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="1.3" sheetId="4" r:id="rId4"/>
     <sheet name="2" sheetId="5" r:id="rId5"/>
     <sheet name="3.1" sheetId="6" r:id="rId6"/>
+    <sheet name="3.2" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>#prueba</t>
   </si>
@@ -119,6 +120,15 @@
   </si>
   <si>
     <t>BBDD</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>Alta coche correcta todos los campos vacíos</t>
+  </si>
+  <si>
+    <t>Después de insertar</t>
   </si>
 </sst>
 </file>
@@ -1949,14 +1959,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>313333</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>37059</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1"/>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>380095</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>106993</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1970,7 +1980,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="368300"/>
-          <a:ext cx="7933333" cy="8323809"/>
+          <a:ext cx="7238095" cy="7657143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1988,9 +1998,128 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>522952</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>46583</xdr:rowOff>
+      <xdr:colOff>618190</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>176788</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="9391650"/>
+          <a:ext cx="7476190" cy="8095238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>161521</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="18415000"/>
+          <a:ext cx="4038600" cy="3292071"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>465809</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>87876</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="368300"/>
+          <a:ext cx="7323809" cy="8190476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>418190</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>40257</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2007,8 +2136,46 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="9391650"/>
-          <a:ext cx="7380952" cy="8333333"/>
+          <a:off x="0" y="9207500"/>
+          <a:ext cx="7276190" cy="8142857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>749346</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="18046700"/>
+          <a:ext cx="3797346" cy="3130550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2286,7 +2453,7 @@
   <dimension ref="A2:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2387,13 +2554,21 @@
       <c r="D7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="4"/>
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -2628,7 +2803,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H105" sqref="H105"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A97"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
       <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
@@ -2636,16 +2842,16 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Análisis User Story modificar componente.
</commit_message>
<xml_diff>
--- a/doc/Pruebas Funcionales/Documento PF.xlsx
+++ b/doc/Pruebas Funcionales/Documento PF.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4420" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4420"/>
   </bookViews>
   <sheets>
     <sheet name="Casos" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t>#prueba</t>
   </si>
@@ -129,6 +129,30 @@
   </si>
   <si>
     <t>Después de insertar</t>
+  </si>
+  <si>
+    <t>Validación nombre componente</t>
+  </si>
+  <si>
+    <t>Validación nombre componente ya existe</t>
+  </si>
+  <si>
+    <t>Validación kilometraje componente</t>
+  </si>
+  <si>
+    <t>Modificar componente</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>Error BBDD modificar componente</t>
+  </si>
+  <si>
+    <t>Correcta modificacion de componente</t>
+  </si>
+  <si>
+    <t>1.5</t>
   </si>
 </sst>
 </file>
@@ -216,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -239,6 +263,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2452,12 +2485,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="28.453125" customWidth="1"/>
     <col min="2" max="2" width="10.90625" style="3"/>
     <col min="3" max="3" width="42.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.26953125" style="5" customWidth="1"/>
@@ -2544,7 +2578,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="8"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
@@ -2559,7 +2593,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="2" t="s">
         <v>30</v>
       </c>
@@ -2569,40 +2603,64 @@
       <c r="D8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="1"/>
+      <c r="A9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="1"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="1"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="1"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="1"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
@@ -2649,8 +2707,9 @@
       <c r="E19" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A3:A7"/>
+  <mergeCells count="2">
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A9:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2834,7 +2893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+    <sheetView topLeftCell="A94" workbookViewId="0">
       <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Cuanod pulso "parametrización" no ejecuta por defecto la busqueda de componentes.
</commit_message>
<xml_diff>
--- a/doc/Pruebas Funcionales/Documento PF.xlsx
+++ b/doc/Pruebas Funcionales/Documento PF.xlsx
@@ -3428,7 +3428,7 @@
   <dimension ref="A2:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3642,7 +3642,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="10" t="s">
         <v>52</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -3655,7 +3655,7 @@
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="2" t="s">
         <v>55</v>
       </c>
@@ -3666,7 +3666,7 @@
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="2" t="s">
         <v>58</v>
       </c>
@@ -3691,9 +3691,10 @@
       <c r="E19" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>